<commit_message>
updated import template file
</commit_message>
<xml_diff>
--- a/client/public/template.xlsx
+++ b/client/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3880B8BF-A555-4AB4-B9C4-93DB636C970D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCDED14-103C-4E0F-A2E3-2BFEF776E485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{147206A8-4F13-4085-8F99-59DDD50A63D6}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,9 +34,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Test</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>University Name</t>
+  </si>
+  <si>
+    <t>Curriculum</t>
+  </si>
+  <si>
+    <t>Academic Year</t>
+  </si>
+  <si>
+    <t>Placement Year</t>
+  </si>
+  <si>
+    <t>Course Year</t>
   </si>
 </sst>
 </file>
@@ -389,15 +403,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6296D558-7F6E-4802-8607-87E76C9D367F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed admin faq page and added response messages to faq apis
</commit_message>
<xml_diff>
--- a/client/public/template.xlsx
+++ b/client/public/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamara\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamara\PlacementSystem\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCDED14-103C-4E0F-A2E3-2BFEF776E485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C61DF9C-4FFF-428F-BE76-78723642100F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{147206A8-4F13-4085-8F99-59DDD50A63D6}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11505" xr2:uid="{147206A8-4F13-4085-8F99-59DDD50A63D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Student Name</t>
   </si>
   <si>
-    <t>University Name</t>
-  </si>
-  <si>
     <t>Curriculum</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>Course Year</t>
+  </si>
+  <si>
+    <t>University Number</t>
   </si>
 </sst>
 </file>
@@ -406,29 +406,29 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>